<commit_message>
Finished sorting taxonomy. Just need to run the body size script and do functional groups
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39938212-A75C-B746-8988-5C2C7364970C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F904F2-5EF8-9742-BF95-B05EC0561C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-11660" windowWidth="27880" windowHeight="28300" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4778" uniqueCount="2850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4780" uniqueCount="2851">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -8596,6 +8596,9 @@
   </si>
   <si>
     <t>Spirotrichea ordo incertae sedis</t>
+  </si>
+  <si>
+    <t>Johansenia</t>
   </si>
 </sst>
 </file>
@@ -21437,10 +21440,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871028EA-29BA-7645-9610-061CA35FE0CC}">
-  <dimension ref="A1:B531"/>
+  <dimension ref="A1:B532"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A526" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B532" sqref="B532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25695,6 +25698,14 @@
       </c>
       <c r="B531" t="s">
         <v>2671</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>2850</v>
+      </c>
+      <c r="B532" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -26021,7 +26032,7 @@
   <dimension ref="A1:B197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished phylogeny, done temporary phylo graph with body sizes
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8232283-8CAF-1C4F-BCB6-B0E8978227B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBBA111-AA81-7C4A-AA83-C8DF40573C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="740" windowWidth="13540" windowHeight="18380" activeTab="6" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="7220" yWindow="740" windowWidth="22180" windowHeight="18380" activeTab="6" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5124" uniqueCount="2959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5126" uniqueCount="2958">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -8790,9 +8790,6 @@
     <t>Diphylleia rotans</t>
   </si>
   <si>
-    <t>Acanthosphaera</t>
-  </si>
-  <si>
     <t>resolved.taxa.name</t>
   </si>
   <si>
@@ -8865,9 +8862,6 @@
     <t>Ochrophyta</t>
   </si>
   <si>
-    <t>Cryptophyta</t>
-  </si>
-  <si>
     <t>Myzozoa</t>
   </si>
   <si>
@@ -8926,6 +8920,9 @@
   </si>
   <si>
     <t>Schizothrix lacustris (species in domain Eukaryota)</t>
+  </si>
+  <si>
+    <t>Acanthosphaera (genus in kingdom Archaeplastida)</t>
   </si>
 </sst>
 </file>
@@ -21687,8 +21684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D62748D-0C36-F54F-B414-4585403A25D9}">
   <dimension ref="A1:B553"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E582" sqref="E582"/>
+    <sheetView topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="A256" sqref="A256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23670,7 +23667,7 @@
         <v>2835</v>
       </c>
       <c r="B247" t="s">
-        <v>425</v>
+        <v>636</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
@@ -26532,10 +26529,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}">
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28048,6 +28045,14 @@
         <v>240</v>
       </c>
     </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>636</v>
+      </c>
+      <c r="B189" t="s">
+        <v>2930</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B189" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28059,7 +28064,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28071,10 +28076,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B1" t="s">
         <v>2914</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2915</v>
       </c>
       <c r="C1" t="s">
         <v>2876</v>
@@ -28118,7 +28123,7 @@
         <v>707845</v>
       </c>
       <c r="D2" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E2" t="s">
         <v>2892</v>
@@ -28139,10 +28144,10 @@
         <v>182</v>
       </c>
       <c r="K2" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L2" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -28156,13 +28161,13 @@
         <v>4016649</v>
       </c>
       <c r="D3" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E3" t="s">
         <v>2893</v>
       </c>
       <c r="F3" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="G3" t="s">
         <v>287</v>
@@ -28177,10 +28182,10 @@
         <v>182</v>
       </c>
       <c r="K3" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L3" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -28194,13 +28199,13 @@
         <v>5409388</v>
       </c>
       <c r="D4" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E4" t="s">
         <v>2894</v>
       </c>
       <c r="F4" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="G4" t="s">
         <v>2693</v>
@@ -28212,18 +28217,18 @@
         <v>97</v>
       </c>
       <c r="J4" t="s">
+        <v>2937</v>
+      </c>
+      <c r="K4" t="s">
         <v>2939</v>
       </c>
-      <c r="K4" t="s">
-        <v>2941</v>
-      </c>
       <c r="L4" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="B5" t="s">
         <v>2895</v>
@@ -28232,7 +28237,7 @@
         <v>5362912</v>
       </c>
       <c r="D5" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F5" t="s">
         <v>2895</v>
@@ -28250,10 +28255,10 @@
         <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L5" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -28261,16 +28266,16 @@
         <v>2886</v>
       </c>
       <c r="B6" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="C6">
         <v>427000</v>
       </c>
       <c r="D6" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="E6" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="F6" t="s">
         <v>2484</v>
@@ -28282,16 +28287,16 @@
         <v>2675</v>
       </c>
       <c r="I6" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="J6" t="s">
         <v>2754</v>
       </c>
       <c r="K6" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L6" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -28305,7 +28310,7 @@
         <v>312183</v>
       </c>
       <c r="D7" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F7" t="s">
         <v>2896</v>
@@ -28320,13 +28325,13 @@
         <v>211</v>
       </c>
       <c r="J7" t="s">
+        <v>2938</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2943</v>
+      </c>
+      <c r="L7" t="s">
         <v>2940</v>
-      </c>
-      <c r="K7" t="s">
-        <v>2945</v>
-      </c>
-      <c r="L7" t="s">
-        <v>2942</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -28340,31 +28345,31 @@
         <v>598957</v>
       </c>
       <c r="D8" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E8" t="s">
         <v>2897</v>
       </c>
       <c r="F8" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="G8" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="H8" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="I8" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="J8" t="s">
+        <v>2938</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2943</v>
+      </c>
+      <c r="L8" t="s">
         <v>2940</v>
-      </c>
-      <c r="K8" t="s">
-        <v>2945</v>
-      </c>
-      <c r="L8" t="s">
-        <v>2942</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -28378,13 +28383,13 @@
         <v>150267</v>
       </c>
       <c r="D9" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E9" t="s">
         <v>497</v>
       </c>
       <c r="F9" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="G9" t="s">
         <v>2632</v>
@@ -28396,13 +28401,13 @@
         <v>211</v>
       </c>
       <c r="J9" t="s">
+        <v>2938</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2943</v>
+      </c>
+      <c r="L9" t="s">
         <v>2940</v>
-      </c>
-      <c r="K9" t="s">
-        <v>2945</v>
-      </c>
-      <c r="L9" t="s">
-        <v>2942</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -28416,7 +28421,7 @@
         <v>4735204</v>
       </c>
       <c r="D10" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F10" t="s">
         <v>2898</v>
@@ -28434,10 +28439,10 @@
         <v>178</v>
       </c>
       <c r="K10" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L10" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -28451,7 +28456,7 @@
         <v>307972</v>
       </c>
       <c r="D11" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F11" t="s">
         <v>2899</v>
@@ -28469,10 +28474,10 @@
         <v>178</v>
       </c>
       <c r="K11" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L11" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -28486,31 +28491,31 @@
         <v>4023445</v>
       </c>
       <c r="D12" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E12" t="s">
         <v>2901</v>
       </c>
       <c r="F12" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="G12" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="H12" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="I12" t="s">
         <v>97</v>
       </c>
       <c r="J12" t="s">
+        <v>2937</v>
+      </c>
+      <c r="K12" t="s">
         <v>2939</v>
       </c>
-      <c r="K12" t="s">
-        <v>2941</v>
-      </c>
       <c r="L12" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -28524,13 +28529,13 @@
         <v>2812112</v>
       </c>
       <c r="D13" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E13" t="s">
         <v>2902</v>
       </c>
       <c r="F13" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="G13" t="s">
         <v>515</v>
@@ -28542,13 +28547,13 @@
         <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="K13" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L13" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -28562,13 +28567,13 @@
         <v>5376792</v>
       </c>
       <c r="D14" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E14" t="s">
         <v>2903</v>
       </c>
       <c r="F14" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="G14" t="s">
         <v>287</v>
@@ -28583,15 +28588,15 @@
         <v>182</v>
       </c>
       <c r="K14" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L14" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="B15" t="s">
         <v>2904</v>
@@ -28600,13 +28605,13 @@
         <v>4016689</v>
       </c>
       <c r="D15" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E15" t="s">
         <v>2904</v>
       </c>
       <c r="F15" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="G15" t="s">
         <v>287</v>
@@ -28621,15 +28626,15 @@
         <v>182</v>
       </c>
       <c r="K15" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L15" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="B16" t="s">
         <v>2909</v>
@@ -28638,7 +28643,7 @@
         <v>6388726</v>
       </c>
       <c r="D16" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E16" t="s">
         <v>2909</v>
@@ -28656,18 +28661,18 @@
         <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="K16" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L16" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
       <c r="B17" t="s">
         <v>2905</v>
@@ -28676,7 +28681,7 @@
         <v>2818322</v>
       </c>
       <c r="D17" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E17" t="s">
         <v>2905</v>
@@ -28694,18 +28699,18 @@
         <v>83</v>
       </c>
       <c r="J17" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="K17" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L17" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="B18" t="s">
         <v>2906</v>
@@ -28714,13 +28719,13 @@
         <v>4016662</v>
       </c>
       <c r="D18" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E18" t="s">
         <v>2906</v>
       </c>
       <c r="F18" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="G18" t="s">
         <v>287</v>
@@ -28735,10 +28740,10 @@
         <v>182</v>
       </c>
       <c r="K18" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L18" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -28752,13 +28757,13 @@
         <v>5153022</v>
       </c>
       <c r="D19" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E19" t="s">
         <v>2907</v>
       </c>
       <c r="F19" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="G19" t="s">
         <v>207</v>
@@ -28773,15 +28778,15 @@
         <v>178</v>
       </c>
       <c r="K19" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L19" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2952</v>
+        <v>2950</v>
       </c>
       <c r="B20" t="s">
         <v>2908</v>
@@ -28790,7 +28795,7 @@
         <v>4016583</v>
       </c>
       <c r="D20" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E20" t="s">
         <v>2908</v>
@@ -28811,15 +28816,15 @@
         <v>182</v>
       </c>
       <c r="K20" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L20" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
       <c r="B21" t="s">
         <v>2338</v>
@@ -28828,13 +28833,13 @@
         <v>4016510</v>
       </c>
       <c r="D21" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E21" t="s">
         <v>2338</v>
       </c>
       <c r="F21" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="G21" t="s">
         <v>2582</v>
@@ -28846,13 +28851,13 @@
         <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="K21" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L21" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -28866,7 +28871,7 @@
         <v>25914</v>
       </c>
       <c r="D22" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F22" t="s">
         <v>418</v>
@@ -28878,21 +28883,21 @@
         <v>420</v>
       </c>
       <c r="I22" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="J22" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="K22" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="L22" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="B23" t="s">
         <v>2862</v>
@@ -28901,7 +28906,7 @@
         <v>7563454</v>
       </c>
       <c r="D23" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F23" t="s">
         <v>2862</v>
@@ -28919,15 +28924,15 @@
         <v>182</v>
       </c>
       <c r="K23" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L23" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="B24" t="s">
         <v>2862</v>
@@ -28936,7 +28941,7 @@
         <v>7563454</v>
       </c>
       <c r="D24" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F24" t="s">
         <v>2862</v>
@@ -28954,15 +28959,15 @@
         <v>182</v>
       </c>
       <c r="K24" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L24" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2954</v>
+        <v>2952</v>
       </c>
       <c r="B25" t="s">
         <v>2910</v>
@@ -28971,7 +28976,7 @@
         <v>4016804</v>
       </c>
       <c r="D25" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E25" t="s">
         <v>2910</v>
@@ -28992,15 +28997,15 @@
         <v>182</v>
       </c>
       <c r="K25" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L25" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="B26" t="s">
         <v>2911</v>
@@ -29009,7 +29014,7 @@
         <v>447081</v>
       </c>
       <c r="D26" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E26" t="s">
         <v>2911</v>
@@ -29030,10 +29035,10 @@
         <v>182</v>
       </c>
       <c r="K26" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="L26" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -29047,7 +29052,7 @@
         <v>606326</v>
       </c>
       <c r="D27" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E27" t="s">
         <v>2891</v>
@@ -29059,19 +29064,19 @@
         <v>636</v>
       </c>
       <c r="H27" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="I27" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="J27" t="s">
+        <v>2938</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2943</v>
+      </c>
+      <c r="L27" t="s">
         <v>2940</v>
-      </c>
-      <c r="K27" t="s">
-        <v>2945</v>
-      </c>
-      <c r="L27" t="s">
-        <v>2942</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -29085,19 +29090,19 @@
         <v>155852</v>
       </c>
       <c r="D28" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F28" t="s">
         <v>2900</v>
       </c>
       <c r="G28" t="s">
-        <v>425</v>
+        <v>636</v>
       </c>
       <c r="H28" t="s">
-        <v>2874</v>
+        <v>2930</v>
       </c>
       <c r="I28" t="s">
-        <v>351</v>
+        <v>2934</v>
       </c>
       <c r="J28" t="s">
         <v>2938</v>
@@ -29106,7 +29111,7 @@
         <v>2943</v>
       </c>
       <c r="L28" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -29114,16 +29119,16 @@
         <v>2832</v>
       </c>
       <c r="B29" t="s">
-        <v>2913</v>
+        <v>2957</v>
       </c>
       <c r="C29">
         <v>6001434</v>
       </c>
       <c r="D29" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="F29" t="s">
-        <v>2913</v>
+        <v>2957</v>
       </c>
       <c r="G29" t="s">
         <v>284</v>
@@ -29138,10 +29143,10 @@
         <v>178</v>
       </c>
       <c r="K29" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L29" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -29155,16 +29160,16 @@
         <v>6000826</v>
       </c>
       <c r="D30" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="E30" t="s">
         <v>826</v>
       </c>
       <c r="F30" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G30" t="s">
         <v>2924</v>
-      </c>
-      <c r="G30" t="s">
-        <v>2925</v>
       </c>
       <c r="H30" t="s">
         <v>99</v>
@@ -29176,10 +29181,10 @@
         <v>178</v>
       </c>
       <c r="K30" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="L30" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in r groups and made tree
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBBA111-AA81-7C4A-AA83-C8DF40573C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F6BDF3-331D-A744-960B-A9563109BD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="740" windowWidth="22180" windowHeight="18380" activeTab="6" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="9500" yWindow="740" windowWidth="19900" windowHeight="18380" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5126" uniqueCount="2958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5156" uniqueCount="2976">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -8923,6 +8923,60 @@
   </si>
   <si>
     <t>Acanthosphaera (genus in kingdom Archaeplastida)</t>
+  </si>
+  <si>
+    <t>Cyclotella k*SpecChar*tzingiana</t>
+  </si>
+  <si>
+    <t>Centrales spp. (5*SpecChar*20 *SpecChar*m)</t>
+  </si>
+  <si>
+    <t>Centrales spp. 5*SpecChar*20 *SpecChar*m</t>
+  </si>
+  <si>
+    <t>Chlorella minut*SpecChar*ssima</t>
+  </si>
+  <si>
+    <t>Cyclotella spp&gt;9*SpecChar*m /stephanodiscus minutulus &gt;7*SpecChar*m</t>
+  </si>
+  <si>
+    <t>Cysts of chrysophyceae (14*SpecChar*)</t>
+  </si>
+  <si>
+    <t>Cyst of chrysophyceaes n*SpecChar*2 (diam. 17,5*SpecChar*m)</t>
+  </si>
+  <si>
+    <t>Cysts of chrysophyceae (30*SpecChar*)</t>
+  </si>
+  <si>
+    <t>Pico chloro esfer*SpecChar**SpecChar*ide 1</t>
+  </si>
+  <si>
+    <t>Pico chloro esfer*SpecChar**SpecChar*ide 2</t>
+  </si>
+  <si>
+    <t>Pico cyano esf*SpecChar**SpecChar*rico 1</t>
+  </si>
+  <si>
+    <t>Pico ni esf*SpecChar**SpecChar*rico</t>
+  </si>
+  <si>
+    <t>Scenedesmus bijugus (turpin) k*SpecChar**SpecChar*tz</t>
+  </si>
+  <si>
+    <t>Cyst of chrysophyceae</t>
+  </si>
+  <si>
+    <t>Cyclotella kutzingiana</t>
+  </si>
+  <si>
+    <t>Stephanodiscus minutulus</t>
+  </si>
+  <si>
+    <t>Cyclotella spp&lt;9*SpecChar*m /stephanodiscus minutulus &lt;7*SpecChar*m</t>
+  </si>
+  <si>
+    <t>Cyst chrysophycee n*SpecChar*1</t>
   </si>
 </sst>
 </file>
@@ -9315,10 +9369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8595BD-503B-484E-A54B-56E3A4EBC765}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10421,6 +10475,126 @@
       </c>
       <c r="B137" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>2958</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2972</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>2961</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>2962</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>2963</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>2964</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>2970</v>
+      </c>
+      <c r="B144" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>2975</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>2959</v>
+      </c>
+      <c r="B147" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>2960</v>
+      </c>
+      <c r="B148" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B149" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>2967</v>
+      </c>
+      <c r="B150" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B151" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>2969</v>
+      </c>
+      <c r="B152" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -28063,7 +28237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E5C4F8-1C01-BF42-B724-4F4BDD8AA479}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated all r groups and replotted phylogeny
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F6BDF3-331D-A744-960B-A9563109BD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08979F97-21EE-E24D-9026-FBEDEC5EC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="740" windowWidth="19900" windowHeight="18380" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="not_genus" sheetId="55" r:id="rId5"/>
     <sheet name="order" sheetId="59" r:id="rId6"/>
     <sheet name="multi_updates" sheetId="60" r:id="rId7"/>
+    <sheet name="cleaned_groups" sheetId="61" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">cleaned_groups!$A$1:$A$290</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">family!$B$1:$B$554</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">multi_updates!$K$1:$K$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">order!$B$1:$B$189</definedName>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5156" uniqueCount="2976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="3393">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -8977,13 +8979,1264 @@
   </si>
   <si>
     <t>Cyst chrysophycee n*SpecChar*1</t>
+  </si>
+  <si>
+    <t>cleaned.taxa.name.gna</t>
+  </si>
+  <si>
+    <t>cleaned.source.gna</t>
+  </si>
+  <si>
+    <t>Cyclotella rhomboideo-elliptica</t>
+  </si>
+  <si>
+    <t>EOL</t>
+  </si>
+  <si>
+    <t>Cyclotella baicalensis</t>
+  </si>
+  <si>
+    <t>Cyclotella ornata</t>
+  </si>
+  <si>
+    <t>Cyclotella minuta</t>
+  </si>
+  <si>
+    <t>Urosolenia eriensis var. morsa</t>
+  </si>
+  <si>
+    <t>Urosolenia eriensis morsa</t>
+  </si>
+  <si>
+    <t>Cyclotella stylorum</t>
+  </si>
+  <si>
+    <t>small Cyclotella</t>
+  </si>
+  <si>
+    <t>Aulacoseira subartica</t>
+  </si>
+  <si>
+    <t>Aulacoseira subarctica</t>
+  </si>
+  <si>
+    <t>Stephanodiscus meyerii</t>
+  </si>
+  <si>
+    <t>Stephanodiscus meyeri</t>
+  </si>
+  <si>
+    <t>Aulacoseira baicalensis</t>
+  </si>
+  <si>
+    <t>Cyclostephanus dubius</t>
+  </si>
+  <si>
+    <t>Cyclostephanos dubius</t>
+  </si>
+  <si>
+    <t>Stephanodiscus neoastrea</t>
+  </si>
+  <si>
+    <t>Stephanodiscus neoastraea</t>
+  </si>
+  <si>
+    <t>Cyclostesphanos</t>
+  </si>
+  <si>
+    <t>Skeletonema cf. subsalsum</t>
+  </si>
+  <si>
+    <t>Skeletonema subsalsum</t>
+  </si>
+  <si>
+    <t>Pennales</t>
+  </si>
+  <si>
+    <t>Eunotia incisa</t>
+  </si>
+  <si>
+    <t>Desmidium laticeps var. quadrangulare</t>
+  </si>
+  <si>
+    <t>Desmidium laticeps quadrangulare</t>
+  </si>
+  <si>
+    <t>Staurastrum cf. chaetoceras</t>
+  </si>
+  <si>
+    <t>Staurastrum chaetoceras</t>
+  </si>
+  <si>
+    <t>Aulacoseira granulata f. curvata</t>
+  </si>
+  <si>
+    <t>Aulacoseira granulata curvata</t>
+  </si>
+  <si>
+    <t>Staurastrum cf. gracile</t>
+  </si>
+  <si>
+    <t>Staurastrum gracile</t>
+  </si>
+  <si>
+    <t>Surirella peisonis</t>
+  </si>
+  <si>
+    <t>Campylodiscus clypeus</t>
+  </si>
+  <si>
+    <t>Aulacoseira ambigua var. ambigua f. spiralis</t>
+  </si>
+  <si>
+    <t>Aulacoseira ambigua</t>
+  </si>
+  <si>
+    <t>Aulacoseira granulata var. granulata</t>
+  </si>
+  <si>
+    <t>Aulacoseira granulata granulata</t>
+  </si>
+  <si>
+    <t>Geminella</t>
+  </si>
+  <si>
+    <t>Catalogue of Life</t>
+  </si>
+  <si>
+    <t>Ulothrichales</t>
+  </si>
+  <si>
+    <t>Mesotaenium chlamydosporum</t>
+  </si>
+  <si>
+    <t>Epiphytic cyanobacteria</t>
+  </si>
+  <si>
+    <t>Rivularia</t>
+  </si>
+  <si>
+    <t>Benthic (epiphytic) desmids and filamentous green algae</t>
+  </si>
+  <si>
+    <t>benthic diatoms</t>
+  </si>
+  <si>
+    <t>Raphidiopsis/Cylindrospermopsis</t>
+  </si>
+  <si>
+    <t>Planktolyngbya circumcreta</t>
+  </si>
+  <si>
+    <t>Limnotrichoideae</t>
+  </si>
+  <si>
+    <t>Jaaginema quadripunctulatum</t>
+  </si>
+  <si>
+    <t>Limnothrix-Planktothrix agardhii</t>
+  </si>
+  <si>
+    <t>Limnothrix amphigranulata</t>
+  </si>
+  <si>
+    <t>Leptolynbgya cf. notata</t>
+  </si>
+  <si>
+    <t>Anabaena minutissima</t>
+  </si>
+  <si>
+    <t>Cylindrospermopsis catemaco</t>
+  </si>
+  <si>
+    <t>Cylindrospermopsis philippinensis</t>
+  </si>
+  <si>
+    <t>Cylindrospermopsis phillippinensis</t>
+  </si>
+  <si>
+    <t>Cylindrospermum cf. muscicola</t>
+  </si>
+  <si>
+    <t>Cylindrospermum muscicola</t>
+  </si>
+  <si>
+    <t>Synechococcus aff. nidulans</t>
+  </si>
+  <si>
+    <t>small chlorelloid cells</t>
+  </si>
+  <si>
+    <t>Carteria complanata</t>
+  </si>
+  <si>
+    <t>Carteria</t>
+  </si>
+  <si>
+    <t>Chlamydomonas depressa</t>
+  </si>
+  <si>
+    <t>Chlamydomonas microsphera</t>
+  </si>
+  <si>
+    <t>Chlamydomonas microsphaera</t>
+  </si>
+  <si>
+    <t>Chlamydomonas passiva</t>
+  </si>
+  <si>
+    <t>Chlamydomonas cf. muriella</t>
+  </si>
+  <si>
+    <t>Chlamydomonas muriella</t>
+  </si>
+  <si>
+    <t>Chloromonas minima</t>
+  </si>
+  <si>
+    <t>Chloromonas</t>
+  </si>
+  <si>
+    <t>Pedimonas</t>
+  </si>
+  <si>
+    <t>Pteromonas variabilis</t>
+  </si>
+  <si>
+    <t>Chlamydomonas planctogloea</t>
+  </si>
+  <si>
+    <t>Chlamydomonas sordida</t>
+  </si>
+  <si>
+    <t>Plagioselmis (Rhodomonas)</t>
+  </si>
+  <si>
+    <t>Monoraphidium cf. nanum</t>
+  </si>
+  <si>
+    <t>Monoraphidium nanum</t>
+  </si>
+  <si>
+    <t>Monoraphidium griffithiii</t>
+  </si>
+  <si>
+    <t>Monoraphidium griffithii</t>
+  </si>
+  <si>
+    <t>Monoraphidium pseudomirabile</t>
+  </si>
+  <si>
+    <t>Monoraphidium pseudomirabilis</t>
+  </si>
+  <si>
+    <t>Keryochlamys styriaca</t>
+  </si>
+  <si>
+    <t>Keriochlamys styriaca</t>
+  </si>
+  <si>
+    <t>Chlorella vulgaris var. autotrophica</t>
+  </si>
+  <si>
+    <t>Chlorella vulgaris autotrophica</t>
+  </si>
+  <si>
+    <t>Synechococcus elegans</t>
+  </si>
+  <si>
+    <t>small sized chrysoflagellates</t>
+  </si>
+  <si>
+    <t>Dynobrioncylindricum</t>
+  </si>
+  <si>
+    <t>Ochromonas cf. viridis</t>
+  </si>
+  <si>
+    <t>Ochromonas viridis</t>
+  </si>
+  <si>
+    <t>Cryptomonas cf. brasiliensis; Cryptomonas pyrenoidifera</t>
+  </si>
+  <si>
+    <t>aff. Teleaulax</t>
+  </si>
+  <si>
+    <t>Cryptomonas acuta</t>
+  </si>
+  <si>
+    <t>Cryptomonas reflexa Gymnodinium</t>
+  </si>
+  <si>
+    <t>Cryptomonas reflexa</t>
+  </si>
+  <si>
+    <t>Cryptomonas cf. marssonii</t>
+  </si>
+  <si>
+    <t>Cryptomonas marssonii</t>
+  </si>
+  <si>
+    <t>Colonial Chlorococcaleans (Botryococcus</t>
+  </si>
+  <si>
+    <t>Coenochlorys</t>
+  </si>
+  <si>
+    <t>Lobocystis planctonica var. mucosa</t>
+  </si>
+  <si>
+    <t>Lobocystis planctonica</t>
+  </si>
+  <si>
+    <t>Eremosphaera tanganyikae</t>
+  </si>
+  <si>
+    <t>Nephroclamys subsolitaria</t>
+  </si>
+  <si>
+    <t>Nephrochlamys subsolitaria</t>
+  </si>
+  <si>
+    <t>Willea wilhelmii</t>
+  </si>
+  <si>
+    <t>Willea vilhelmii</t>
+  </si>
+  <si>
+    <t>Oocytis borgei</t>
+  </si>
+  <si>
+    <t>Oocystis borgei</t>
+  </si>
+  <si>
+    <t>Eutetramorus fottiii</t>
+  </si>
+  <si>
+    <t>Eutetramorus fottii</t>
+  </si>
+  <si>
+    <t>Ketablepharis</t>
+  </si>
+  <si>
+    <t>Pediastrum biwae</t>
+  </si>
+  <si>
+    <t>Tetraedron tumidulum</t>
+  </si>
+  <si>
+    <t>Micratinium</t>
+  </si>
+  <si>
+    <t>Scenedesmus acuminatum</t>
+  </si>
+  <si>
+    <t>Scenedesmus acuminatus</t>
+  </si>
+  <si>
+    <t>Scenedesmus acuminatum var. bernardii</t>
+  </si>
+  <si>
+    <t>Scenedesmus acuminatus bernardii</t>
+  </si>
+  <si>
+    <t>Scenedesmus arcuatum</t>
+  </si>
+  <si>
+    <t>Scenedesmus arcuatus</t>
+  </si>
+  <si>
+    <t>Scenedesmus quadricauda var. parvus</t>
+  </si>
+  <si>
+    <t>Scenedesmus quadricauda parvus</t>
+  </si>
+  <si>
+    <t>Tetraedron gracilis</t>
+  </si>
+  <si>
+    <t>Tetraedron gracile</t>
+  </si>
+  <si>
+    <t>Tetraedron mediocris</t>
+  </si>
+  <si>
+    <t>Tetraedron victoriae</t>
+  </si>
+  <si>
+    <t>Oocystis marina</t>
+  </si>
+  <si>
+    <t>Goniochlorys mutica</t>
+  </si>
+  <si>
+    <t>Goniochloris mutica</t>
+  </si>
+  <si>
+    <t>Tetraedron trigonium</t>
+  </si>
+  <si>
+    <t>Ankistrodesmus/Monoraphidium</t>
+  </si>
+  <si>
+    <t>Gloeocapsa punctata</t>
+  </si>
+  <si>
+    <t>Anabaena cf. circinalis</t>
+  </si>
+  <si>
+    <t>Anabaena circinalis</t>
+  </si>
+  <si>
+    <t>Anabaena cf. scheremetievi</t>
+  </si>
+  <si>
+    <t>Anabaena scheremetievi</t>
+  </si>
+  <si>
+    <t>Anabaena cf. solitaria</t>
+  </si>
+  <si>
+    <t>Anabaena perturbata</t>
+  </si>
+  <si>
+    <t>Anabaena elenkinii</t>
+  </si>
+  <si>
+    <t>Anabaena tanganyikae</t>
+  </si>
+  <si>
+    <t>Anabaena tanganykae</t>
+  </si>
+  <si>
+    <t>Aphanizomenon cf. flos-aquae</t>
+  </si>
+  <si>
+    <t>Aphanizomenon flos-aquae</t>
+  </si>
+  <si>
+    <t>Anabaena cf. aphanizomenoides</t>
+  </si>
+  <si>
+    <t>Anabaena aphanizomendoides</t>
+  </si>
+  <si>
+    <t>Aphanizomenon aphanizomenoides</t>
+  </si>
+  <si>
+    <t>Anabaena group</t>
+  </si>
+  <si>
+    <t>Anabaena sphaerica</t>
+  </si>
+  <si>
+    <t>Ceratium-Snowella</t>
+  </si>
+  <si>
+    <t>Peridinium gatunense</t>
+  </si>
+  <si>
+    <t>Peridiniopsis durandi</t>
+  </si>
+  <si>
+    <t>Peridinium cf. cinctum</t>
+  </si>
+  <si>
+    <t>Peridinium cinctum</t>
+  </si>
+  <si>
+    <t>Coelomoron tropicalis</t>
+  </si>
+  <si>
+    <t>Coelomoron tropicale</t>
+  </si>
+  <si>
+    <t>Microcystis lamelliformis</t>
+  </si>
+  <si>
+    <t>Tabellaria flocculosa var. fenestrata</t>
+  </si>
+  <si>
+    <t>Isocystis pallida</t>
+  </si>
+  <si>
+    <t>Leptolyngbya tenue</t>
+  </si>
+  <si>
+    <t>Leptolyngbya antartica</t>
+  </si>
+  <si>
+    <t>Leptolyngbya antarctica</t>
+  </si>
+  <si>
+    <t>Chromatium</t>
+  </si>
+  <si>
+    <t>Pyrobotrys</t>
+  </si>
+  <si>
+    <t>Beggiatoa alba</t>
+  </si>
+  <si>
+    <t>Vacuolaria tropicalis</t>
+  </si>
+  <si>
+    <t>Trachelomonas sculpta</t>
+  </si>
+  <si>
+    <t>Trachelomonas hispida var. hispida</t>
+  </si>
+  <si>
+    <t>Trachelomonas hispida hispida</t>
+  </si>
+  <si>
+    <t>Trachelomonas reticollis</t>
+  </si>
+  <si>
+    <t>Trachelomonas recticollis</t>
+  </si>
+  <si>
+    <t>Dimorphococcus</t>
+  </si>
+  <si>
+    <t>Gonynostomum</t>
+  </si>
+  <si>
+    <t>Heterosigma cf. akashiwo</t>
+  </si>
+  <si>
+    <t>Heterosigma akashiwo</t>
+  </si>
+  <si>
+    <t>Romeria chlorina</t>
+  </si>
+  <si>
+    <t>Chlorella + Choricysits</t>
+  </si>
+  <si>
+    <t>Merismopedia cf. hyalina</t>
+  </si>
+  <si>
+    <t>Merismopedia hyalina</t>
+  </si>
+  <si>
+    <t>cf Mantellum sp.</t>
+  </si>
+  <si>
+    <t>Cylindrospermum Bourget03</t>
+  </si>
+  <si>
+    <t>Cell of Dinobryon</t>
+  </si>
+  <si>
+    <t>Centric (Cyclotella + Stephanodiscus)</t>
+  </si>
+  <si>
+    <t>Centric &lt;10µm</t>
+  </si>
+  <si>
+    <t>cf. Katodinium fongiforme</t>
+  </si>
+  <si>
+    <t>Geminella subtilissima</t>
+  </si>
+  <si>
+    <t>Stomatocyst FR1</t>
+  </si>
+  <si>
+    <t>Cyst 1 of Chrysophyceae</t>
+  </si>
+  <si>
+    <t>Oedogonium large cell Bourget03</t>
+  </si>
+  <si>
+    <t>Cyst Chrysophycee N°1</t>
+  </si>
+  <si>
+    <t>Centric &gt;10µm</t>
+  </si>
+  <si>
+    <t>Cyst 2 of Chrysophyceae</t>
+  </si>
+  <si>
+    <t>Cyst of Dinobryon</t>
+  </si>
+  <si>
+    <t>micro Chlorophyceae</t>
+  </si>
+  <si>
+    <t>Cysts of Chrysophyceae (14µ)</t>
+  </si>
+  <si>
+    <t>Staurastrum sp. Annecy 2004</t>
+  </si>
+  <si>
+    <t>Cyst of Chrysophyceaes N°2 (diam. 17,5µm)</t>
+  </si>
+  <si>
+    <t>Cyst of Ceratium hirundinella</t>
+  </si>
+  <si>
+    <t>Cysts of Chrysophyceae (30µ)</t>
+  </si>
+  <si>
+    <t>Actinastrum</t>
+  </si>
+  <si>
+    <t>Aphanocapsa/Aphanothece</t>
+  </si>
+  <si>
+    <t>Chromulina/Chrysococcus</t>
+  </si>
+  <si>
+    <t>Chrysophyceae/Xanthophyceae</t>
+  </si>
+  <si>
+    <t>Closterium/Closteriopsis</t>
+  </si>
+  <si>
+    <t>Coelomorom microcystoides/Eucapsis parallelepipedon</t>
+  </si>
+  <si>
+    <t>Coelomoron/Woronchinia 2</t>
+  </si>
+  <si>
+    <t>Coenocystis/Oocystis</t>
+  </si>
+  <si>
+    <t>Diatomococcus/Tetralitris</t>
+  </si>
+  <si>
+    <t>Dinobryon divergens Imhof</t>
+  </si>
+  <si>
+    <t>Dinobryon divergens</t>
+  </si>
+  <si>
+    <t>Dinobryon sertularia Ehr</t>
+  </si>
+  <si>
+    <t>Dinobryon sertularia</t>
+  </si>
+  <si>
+    <t>Dinoflagelado/Peridinium</t>
+  </si>
+  <si>
+    <t>Durinskia sp/Dinoflagelado</t>
+  </si>
+  <si>
+    <t>Elakatothrix americana Wille</t>
+  </si>
+  <si>
+    <t>Elakatothrix americana</t>
+  </si>
+  <si>
+    <t>Elakatothrix gelatinosa Wille</t>
+  </si>
+  <si>
+    <t>Elakatothrix gelatinosa</t>
+  </si>
+  <si>
+    <t>Elakatotrix americana X cel</t>
+  </si>
+  <si>
+    <t>Entomoneis alata (Ehr) Kutz</t>
+  </si>
+  <si>
+    <t>Entomoneis alata</t>
+  </si>
+  <si>
+    <t>Epithemia zebra (Ehr)Kutz</t>
+  </si>
+  <si>
+    <t>Epithemia zebra</t>
+  </si>
+  <si>
+    <t>Euglena clabata Skuja</t>
+  </si>
+  <si>
+    <t>Euglena clavata</t>
+  </si>
+  <si>
+    <t>Euglena oxyuris Schmarda</t>
+  </si>
+  <si>
+    <t>Euglena oxyuris</t>
+  </si>
+  <si>
+    <t>Euglena viridis Ehr</t>
+  </si>
+  <si>
+    <t>Euglena viridis</t>
+  </si>
+  <si>
+    <t>Eutetramorus fotti (Hind) Kom</t>
+  </si>
+  <si>
+    <t>Eutetramorus planctonicus Ehr</t>
+  </si>
+  <si>
+    <t>Eutetramorus planctonicus</t>
+  </si>
+  <si>
+    <t>Eutetramorus tetrasporus Kom</t>
+  </si>
+  <si>
+    <t>Eutetramorus tetrasporus</t>
+  </si>
+  <si>
+    <t>Fragilaria construens (Ehr) Grunow</t>
+  </si>
+  <si>
+    <t>Fragilaria/Synedra</t>
+  </si>
+  <si>
+    <t>Geminella/Binuclearia</t>
+  </si>
+  <si>
+    <t>Glaucospira laxissima/Spirulina</t>
+  </si>
+  <si>
+    <t>Gloeocystis gigas X ORG</t>
+  </si>
+  <si>
+    <t>Golenkinia/ Golenkiniopsis 1</t>
+  </si>
+  <si>
+    <t>Golenkinia/ Golenkiniopsis 2</t>
+  </si>
+  <si>
+    <t>Golenkinia/Golenkiniopsis sp3</t>
+  </si>
+  <si>
+    <t>Gomphonema clavatum Ehr</t>
+  </si>
+  <si>
+    <t>Gomphonema clavatum</t>
+  </si>
+  <si>
+    <t>Gomphosphaeria nageliana (Unger)Lemm</t>
+  </si>
+  <si>
+    <t>Gomphosphaeria naegeliana</t>
+  </si>
+  <si>
+    <t>Goniochloris mutica (ABraun) Fott</t>
+  </si>
+  <si>
+    <t>Gyrosigma obtusatum (Sulliv&amp; Wormley) Boyer</t>
+  </si>
+  <si>
+    <t>Gyrosigma obtusatum</t>
+  </si>
+  <si>
+    <t>Gyrosigma scalpoides (Rabh) Cleve</t>
+  </si>
+  <si>
+    <t>Gyrosigma scalproides</t>
+  </si>
+  <si>
+    <t>Hemiselmis simplex Butcher</t>
+  </si>
+  <si>
+    <t>Hemiselmis simplex</t>
+  </si>
+  <si>
+    <t>Kirchneriella irregularis (GMSmith) Kors</t>
+  </si>
+  <si>
+    <t>Kirchneriella irregularis</t>
+  </si>
+  <si>
+    <t>Lagerheimia subalsa Lemm</t>
+  </si>
+  <si>
+    <t>Lagerheimia wratislaviensis Schroeder</t>
+  </si>
+  <si>
+    <t>Lagerheimia wratislaviensis</t>
+  </si>
+  <si>
+    <t>Lagherimia subsalsa Lemm</t>
+  </si>
+  <si>
+    <t>Lepocinclis ovum (Ehr) Lemm</t>
+  </si>
+  <si>
+    <t>Lepocinclis ovum</t>
+  </si>
+  <si>
+    <t>Mallomonas akrokomos Ruttner</t>
+  </si>
+  <si>
+    <t>Mallomonas akrokomos</t>
+  </si>
+  <si>
+    <t>Melosira varians C Agardh</t>
+  </si>
+  <si>
+    <t>Melosira varians</t>
+  </si>
+  <si>
+    <t>Merismopedia  glauca (Ehr)</t>
+  </si>
+  <si>
+    <t>Merismopedia glauca</t>
+  </si>
+  <si>
+    <t>Merismopedia elegans A Braun</t>
+  </si>
+  <si>
+    <t>Merismopedia glauca (Ehr) Nageli</t>
+  </si>
+  <si>
+    <t>Merismopedia tenuissima Lemm</t>
+  </si>
+  <si>
+    <t>Merismopedia tenuissima</t>
+  </si>
+  <si>
+    <t>Micractinium pusillum Fres</t>
+  </si>
+  <si>
+    <t>Micractinium pusillum</t>
+  </si>
+  <si>
+    <t>Monoraphidium arcuatum (Kors) Hind</t>
+  </si>
+  <si>
+    <t>Monoraphidium circinale (Nyg) Nyg</t>
+  </si>
+  <si>
+    <t>Monoraphidium circinale</t>
+  </si>
+  <si>
+    <t>Monoraphidium contortum (Thur) Kom  Legn</t>
+  </si>
+  <si>
+    <t>Monoraphidium minutum Kom Legn</t>
+  </si>
+  <si>
+    <t>Monoraphidium minutum</t>
+  </si>
+  <si>
+    <t>Monoraphidium tortile (West &amp; West) Kom Legn</t>
+  </si>
+  <si>
+    <t>Monoraphidium tortile</t>
+  </si>
+  <si>
+    <t>Nephrocytium agardhianum Nag</t>
+  </si>
+  <si>
+    <t>Nephrocytium agardhianum</t>
+  </si>
+  <si>
+    <t>Nephroselmis angulata (Kors) Skuja</t>
+  </si>
+  <si>
+    <t>Nephroselmis angulata</t>
+  </si>
+  <si>
+    <t>Nephroselmis minuta (NCarter) H P</t>
+  </si>
+  <si>
+    <t>Nephroselmis minuta</t>
+  </si>
+  <si>
+    <t>Nitzschia acicularis WSmith</t>
+  </si>
+  <si>
+    <t>Nitzschia acicularis</t>
+  </si>
+  <si>
+    <t>Nitzschia fonticola Grun</t>
+  </si>
+  <si>
+    <t>Nitzschia fonticola</t>
+  </si>
+  <si>
+    <t>Nitzschia reversa WSmith</t>
+  </si>
+  <si>
+    <t>Nitzschia reversa</t>
+  </si>
+  <si>
+    <t>Nitzschia sigmoidea (Nizsch)W Smith</t>
+  </si>
+  <si>
+    <t>Nitzschia sigmoidea</t>
+  </si>
+  <si>
+    <t>Nitzschia solita Hust</t>
+  </si>
+  <si>
+    <t>Nitzschia solita</t>
+  </si>
+  <si>
+    <t>Nodularia spumigena Mert</t>
+  </si>
+  <si>
+    <t>Nodularia spumigena</t>
+  </si>
+  <si>
+    <t>Nodularia spumigena Mertens ex Bornet et Flahault</t>
+  </si>
+  <si>
+    <t>Oocystis lacustris Chod</t>
+  </si>
+  <si>
+    <t>Oocystis lacustris</t>
+  </si>
+  <si>
+    <t>Oocystis marsonii Lemm</t>
+  </si>
+  <si>
+    <t>Oocystis marssonii</t>
+  </si>
+  <si>
+    <t>Oocystis natans (Lemm) Playf</t>
+  </si>
+  <si>
+    <t>Oocystis natans</t>
+  </si>
+  <si>
+    <t>Oocystis parva WWest &amp; GSWest</t>
+  </si>
+  <si>
+    <t>Oocystis parva</t>
+  </si>
+  <si>
+    <t>Oocystis submarina Lagerh</t>
+  </si>
+  <si>
+    <t>Oocystis submarina</t>
+  </si>
+  <si>
+    <t>Oscillatoria curviceps Agard</t>
+  </si>
+  <si>
+    <t>Oscillatoria curviceps</t>
+  </si>
+  <si>
+    <t>Pediastrum duplex Meyen</t>
+  </si>
+  <si>
+    <t>Pediastrum duplex</t>
+  </si>
+  <si>
+    <t>Pediastrum tetras (Ehrenb)Ralfs</t>
+  </si>
+  <si>
+    <t>Pediastrum tetras</t>
+  </si>
+  <si>
+    <t>Peridiniopsis borgei Lemm</t>
+  </si>
+  <si>
+    <t>Peridiniopsis borgei</t>
+  </si>
+  <si>
+    <t>Peridinium willei Huif Kass</t>
+  </si>
+  <si>
+    <t>Peridinium willei</t>
+  </si>
+  <si>
+    <t>Peridinium/Gyrodinium</t>
+  </si>
+  <si>
+    <t>Phacotus minusculus Bourr</t>
+  </si>
+  <si>
+    <t>Phacotus minusculus</t>
+  </si>
+  <si>
+    <t>Phacus acuminatus Stokes</t>
+  </si>
+  <si>
+    <t>Phacus acuminatus</t>
+  </si>
+  <si>
+    <t>Phacus brevicaudatus (Klebs) Lemm</t>
+  </si>
+  <si>
+    <t>Phacus brevicaudatus</t>
+  </si>
+  <si>
+    <t>Phacus curvicauda Swir</t>
+  </si>
+  <si>
+    <t>Phacus curvicauda</t>
+  </si>
+  <si>
+    <t>Phacus longicauda (Ehr) Duj</t>
+  </si>
+  <si>
+    <t>Phacus longicauda</t>
+  </si>
+  <si>
+    <t>Phacus triqueter (Ehr) Duj</t>
+  </si>
+  <si>
+    <t>Phacus triqueter</t>
+  </si>
+  <si>
+    <t>Pico Chloro flagelado 1</t>
+  </si>
+  <si>
+    <t>Pico Chloro gota</t>
+  </si>
+  <si>
+    <t>Pico Chryso 2</t>
+  </si>
+  <si>
+    <t>Pico Chryso 3</t>
+  </si>
+  <si>
+    <t>Pico Chryso 4</t>
+  </si>
+  <si>
+    <t>Pico Chryso fla 1</t>
+  </si>
+  <si>
+    <t>Pico cyano (&lt;1um)</t>
+  </si>
+  <si>
+    <t>Pica cyana</t>
+  </si>
+  <si>
+    <t>Pico NI esferoide</t>
+  </si>
+  <si>
+    <t>Pico NI flagelado 1</t>
+  </si>
+  <si>
+    <t>Pinnularia major Rabh</t>
+  </si>
+  <si>
+    <t>Pinnularia major</t>
+  </si>
+  <si>
+    <t>Plagioselmis lacustris (Pasch &amp; Rutt) Javor</t>
+  </si>
+  <si>
+    <t>Plagioselmis lacustris</t>
+  </si>
+  <si>
+    <t>Planktothrix agardhii Gom</t>
+  </si>
+  <si>
+    <t>Planktothrix agardhii</t>
+  </si>
+  <si>
+    <t>Pseudanabaena catenata Lauterborn</t>
+  </si>
+  <si>
+    <t>Pseudodictyosphaerium Jurisii</t>
+  </si>
+  <si>
+    <t>Pseudodictyosphaerium</t>
+  </si>
+  <si>
+    <t>Pseudokephyrion spirale Gerl Schmidt</t>
+  </si>
+  <si>
+    <t>Pseudokephyrion spirale</t>
+  </si>
+  <si>
+    <t>Pteromonas limnetica Hort</t>
+  </si>
+  <si>
+    <t>Pteromonas limnetica</t>
+  </si>
+  <si>
+    <t>Pteromonas sp Rara</t>
+  </si>
+  <si>
+    <t>Pteromonas</t>
+  </si>
+  <si>
+    <t>Pyramimonas minima Pasch</t>
+  </si>
+  <si>
+    <t>Pyramimonas minima</t>
+  </si>
+  <si>
+    <t>Quadrigula closterioides (Bohl) Printz</t>
+  </si>
+  <si>
+    <t>Quadrigula closterioides</t>
+  </si>
+  <si>
+    <t>Quadrigula quaternata (W&amp;GS West) Printz</t>
+  </si>
+  <si>
+    <t>Quadrigula quaternata</t>
+  </si>
+  <si>
+    <t>Rhodomonas minuta Skuja</t>
+  </si>
+  <si>
+    <t>Rhodomonas minuta</t>
+  </si>
+  <si>
+    <t>Scenedesmums linearis Kom</t>
+  </si>
+  <si>
+    <t>Scenedesmus linearis</t>
+  </si>
+  <si>
+    <t>Scenedesmus bicaudatus Dedus</t>
+  </si>
+  <si>
+    <t>Scenedesmus bicaudatus</t>
+  </si>
+  <si>
+    <t>Scenedesmus ecornis (Ehr) Chod</t>
+  </si>
+  <si>
+    <t>Scenedesmus ecornis</t>
+  </si>
+  <si>
+    <t>Scenedesmus intermedius Chod</t>
+  </si>
+  <si>
+    <t>Skeletonema potamos (Weber) Hasle</t>
+  </si>
+  <si>
+    <t>Skeletonema potamos</t>
+  </si>
+  <si>
+    <t>Skeletonema subsalsum (Cleve Euler) Bethge</t>
+  </si>
+  <si>
+    <t>Spermatozopsis exsultans Kors</t>
+  </si>
+  <si>
+    <t>Spermatozopsis exsultans</t>
+  </si>
+  <si>
+    <t>Sphaerocavum/Mpanniformis (isolada)</t>
+  </si>
+  <si>
+    <t>Sphaerocystis cf schroeteri X ORG</t>
+  </si>
+  <si>
+    <t>Sphaerocystis schoeteri Chod</t>
+  </si>
+  <si>
+    <t>Staurastrum gracile Ralfs</t>
+  </si>
+  <si>
+    <t>Staurastrum leptocladum Nordst</t>
+  </si>
+  <si>
+    <t>Staurastrum leptocladum</t>
+  </si>
+  <si>
+    <t>Staurastrum paradoxum Meyen</t>
+  </si>
+  <si>
+    <t>Staurastrum paradoxum</t>
+  </si>
+  <si>
+    <t>Staurastrum quadricauda (Turp) Breb</t>
+  </si>
+  <si>
+    <t>Staurastrum rotula Nordst</t>
+  </si>
+  <si>
+    <t>Staurastrum rotula</t>
+  </si>
+  <si>
+    <t>Staurastrum sebaldi var ornatum Nordst</t>
+  </si>
+  <si>
+    <t>Staurastrum sebaldi ornatum</t>
+  </si>
+  <si>
+    <t>Strombomonas fluviatilis (Lemm) Defl</t>
+  </si>
+  <si>
+    <t>Strombomonas fluviatilis</t>
+  </si>
+  <si>
+    <t>Strombomonas scabra (Playf) Tell &amp; Conf</t>
+  </si>
+  <si>
+    <t>Strombomonas scabra</t>
+  </si>
+  <si>
+    <t>Synedra acus Kuetz</t>
+  </si>
+  <si>
+    <t>Synedra acus</t>
+  </si>
+  <si>
+    <t>Synedra ulna (Nitzsch) Ehr</t>
+  </si>
+  <si>
+    <t>Synedra ulna</t>
+  </si>
+  <si>
+    <t>Tetraedron minimun (A Br) Hansg</t>
+  </si>
+  <si>
+    <t>Tetraedron</t>
+  </si>
+  <si>
+    <t>Tetrastrum glabrum (Roll) Ahlstrom &amp; Tiffany</t>
+  </si>
+  <si>
+    <t>Tetrastrum glabrum</t>
+  </si>
+  <si>
+    <t>Tetrastrum staurogeniaeforme (Schroed) Lemm</t>
+  </si>
+  <si>
+    <t>Tetrastrum staurogeniaeforme</t>
+  </si>
+  <si>
+    <t>Trachelomonas rugulosa Stein</t>
+  </si>
+  <si>
+    <t>Trachelomonas rugulosa</t>
+  </si>
+  <si>
+    <t>Trachelomonas volvocina Ehr</t>
+  </si>
+  <si>
+    <t>Trachelomonas volvocina</t>
+  </si>
+  <si>
+    <t>Trachelomonas volvocina Ehr var volvocina Ehr</t>
+  </si>
+  <si>
+    <t>Trachelomonas volvocina volvocina</t>
+  </si>
+  <si>
+    <t>TrybionelLa vitoriae</t>
+  </si>
+  <si>
+    <t>Urosolenia eriensis Smith</t>
+  </si>
+  <si>
+    <t>Urosolenia eriensis</t>
+  </si>
+  <si>
+    <t>Urosolenia longiseta Zacharias</t>
+  </si>
+  <si>
+    <t>Urosolenia longiseta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9009,6 +10262,19 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -9030,11 +10296,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9371,8 +10639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8595BD-503B-484E-A54B-56E3A4EBC765}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView topLeftCell="A143" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10607,8 +11875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286B08F2-9C4E-3A43-A7E5-D98B8AC33438}">
   <dimension ref="A1:C665"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14011,7 +15279,7 @@
         <v>1534</v>
       </c>
       <c r="B309" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C309" t="s">
         <v>9</v>
@@ -14022,7 +15290,7 @@
         <v>1535</v>
       </c>
       <c r="B310" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C310" t="s">
         <v>9</v>
@@ -14033,7 +15301,7 @@
         <v>1536</v>
       </c>
       <c r="B311" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C311" t="s">
         <v>9</v>
@@ -14044,7 +15312,7 @@
         <v>1537</v>
       </c>
       <c r="B312" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C312" t="s">
         <v>9</v>
@@ -14055,7 +15323,7 @@
         <v>1538</v>
       </c>
       <c r="B313" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C313" t="s">
         <v>9</v>
@@ -14066,7 +15334,7 @@
         <v>1539</v>
       </c>
       <c r="B314" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C314" t="s">
         <v>9</v>
@@ -14077,7 +15345,7 @@
         <v>1540</v>
       </c>
       <c r="B315" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C315" t="s">
         <v>9</v>
@@ -14088,7 +15356,7 @@
         <v>1541</v>
       </c>
       <c r="B316" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C316" t="s">
         <v>9</v>
@@ -14099,7 +15367,7 @@
         <v>1542</v>
       </c>
       <c r="B317" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C317" t="s">
         <v>9</v>
@@ -14110,7 +15378,7 @@
         <v>1543</v>
       </c>
       <c r="B318" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C318" t="s">
         <v>9</v>
@@ -14121,7 +15389,7 @@
         <v>1544</v>
       </c>
       <c r="B319" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C319" t="s">
         <v>9</v>
@@ -14132,7 +15400,7 @@
         <v>1545</v>
       </c>
       <c r="B320" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C320" t="s">
         <v>9</v>
@@ -14143,7 +15411,7 @@
         <v>1546</v>
       </c>
       <c r="B321" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C321" t="s">
         <v>9</v>
@@ -14154,7 +15422,7 @@
         <v>1547</v>
       </c>
       <c r="B322" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C322" t="s">
         <v>9</v>
@@ -17608,7 +18876,7 @@
         <v>1409</v>
       </c>
       <c r="B636" t="s">
-        <v>83</v>
+        <v>2999</v>
       </c>
       <c r="C636" t="s">
         <v>9</v>
@@ -26300,10 +27568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716ADC0-6E42-9D4D-83DC-88C472B153C8}">
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A78"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26694,6 +27962,11 @@
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>2999</v>
       </c>
     </row>
   </sheetData>
@@ -29365,4 +30638,2939 @@
   <autoFilter ref="K1:K30" xr:uid="{C5E5C4F8-1C01-BF42-B724-4F4BDD8AA479}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F58C34-D174-0941-8CA4-E78200493E15}">
+  <dimension ref="A1:C290"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2976</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2978</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2980</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2980</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2981</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2981</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2982</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2984</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>2985</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>2988</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2990</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>2991</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>2991</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2993</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>2995</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>2997</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>2998</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>2999</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>3000</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>3002</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>3006</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3008</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>3009</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>3009</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>3010</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>3011</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>3012</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>3015</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>3017</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>3018</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>3020</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>3020</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>3023</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>3024</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>3024</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>3026</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>3027</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>3030</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>3031</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>3032</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>3032</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>3035</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>3040</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>3042</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>3045</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>3047</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>3048</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>3049</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>3050</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>3050</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>3051</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>3052</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>3054</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>3055</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>3056</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>3058</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>3061</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>3062</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>2874</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>2874</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>3064</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>3065</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>3066</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>3067</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>3068</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>3069</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>3070</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>3070</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>3071</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>3072</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>3073</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>3074</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>3075</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>3076</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>3077</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>3078</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>3079</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>3082</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>3083</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>3087</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>3089</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>3089</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>3090</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>3090</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>3092</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>3097</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>3099</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>3100</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>3101</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>3102</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>3103</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>3103</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>3104</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>3105</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>3109</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>3111</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>3114</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>3115</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>3117</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>3118</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>3119</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>3120</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>3122</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>3123</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>3125</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>3126</v>
+      </c>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>3127</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>3128</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>3128</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
+        <v>3129</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
+        <v>3134</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>3135</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>3136</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>3136</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>3137</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>3138</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>3139</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>3139</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>3141</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>3141</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>3142</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>3143</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>3146</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>3147</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
+        <v>3150</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>3151</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>3152</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
+        <v>3153</v>
+      </c>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>3155</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="4" t="s">
+        <v>3156</v>
+      </c>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="4" t="s">
+        <v>3158</v>
+      </c>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>3159</v>
+      </c>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="4" t="s">
+        <v>3161</v>
+      </c>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>3162</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="4" t="s">
+        <v>3163</v>
+      </c>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="4" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="s">
+        <v>3165</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="4" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>3167</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="4" t="s">
+        <v>3168</v>
+      </c>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="4" t="s">
+        <v>3169</v>
+      </c>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="4" t="s">
+        <v>3170</v>
+      </c>
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="4" t="s">
+        <v>3171</v>
+      </c>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="4" t="s">
+        <v>3172</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="4" t="s">
+        <v>3173</v>
+      </c>
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="4" t="s">
+        <v>3174</v>
+      </c>
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="4" t="s">
+        <v>3175</v>
+      </c>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="4" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="4" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="4" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="4" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
+        <v>3178</v>
+      </c>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="4" t="s">
+        <v>3179</v>
+      </c>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="4" t="s">
+        <v>3180</v>
+      </c>
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="4" t="s">
+        <v>3181</v>
+      </c>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="4" t="s">
+        <v>3182</v>
+      </c>
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="4" t="s">
+        <v>3183</v>
+      </c>
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="4" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="4" t="s">
+        <v>3185</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>3186</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="4" t="s">
+        <v>3187</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="4" t="s">
+        <v>3189</v>
+      </c>
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="4" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="4" t="s">
+        <v>3191</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>3192</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>3193</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>3195</v>
+      </c>
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>3197</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="4" t="s">
+        <v>3198</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>3200</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>3201</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="4" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>3203</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>3204</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>3205</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>3206</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>3087</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>3207</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>3208</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>3209</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>3210</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>3212</v>
+      </c>
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>3213</v>
+      </c>
+      <c r="B182" s="5"/>
+      <c r="C182" s="5"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>3214</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>3215</v>
+      </c>
+      <c r="B184" s="5"/>
+      <c r="C184" s="5"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>3216</v>
+      </c>
+      <c r="B185" s="5"/>
+      <c r="C185" s="5"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="4" t="s">
+        <v>3217</v>
+      </c>
+      <c r="B186" s="5"/>
+      <c r="C186" s="5"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="4" t="s">
+        <v>3218</v>
+      </c>
+      <c r="B187" s="5"/>
+      <c r="C187" s="5"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="4" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>3220</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>3221</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>3222</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
+        <v>3223</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
+        <v>3224</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>3225</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="4" t="s">
+        <v>3226</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>3227</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
+        <v>3228</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>3229</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="4" t="s">
+        <v>3230</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>3231</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
+        <v>3232</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C195" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
+        <v>3233</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>3234</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>3235</v>
+      </c>
+      <c r="B197" s="5"/>
+      <c r="C197" s="5"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="4" t="s">
+        <v>3236</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>3237</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="4" t="s">
+        <v>3238</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>3239</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="4" t="s">
+        <v>3240</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>3241</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="4" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>3243</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="4" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>2910</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="4" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>3243</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="4" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>3247</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="4" t="s">
+        <v>3248</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>3249</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="4" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="4" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="4" t="s">
+        <v>3250</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="4" t="s">
+        <v>3251</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>3252</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="4" t="s">
+        <v>3253</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="4" t="s">
+        <v>3254</v>
+      </c>
+      <c r="B211" s="5" t="s">
+        <v>3255</v>
+      </c>
+      <c r="C211" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="4" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>3257</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="4" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>3259</v>
+      </c>
+      <c r="C213" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="4" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>3261</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="4" t="s">
+        <v>3262</v>
+      </c>
+      <c r="B215" s="5" t="s">
+        <v>3263</v>
+      </c>
+      <c r="C215" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="4" t="s">
+        <v>3264</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>3265</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="4" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>3267</v>
+      </c>
+      <c r="C217" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="4" t="s">
+        <v>3268</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>3269</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="4" t="s">
+        <v>3270</v>
+      </c>
+      <c r="B219" s="5" t="s">
+        <v>3271</v>
+      </c>
+      <c r="C219" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="4" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>3273</v>
+      </c>
+      <c r="C220" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" s="4" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>3275</v>
+      </c>
+      <c r="C221" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="4" t="s">
+        <v>3276</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>3275</v>
+      </c>
+      <c r="C222" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>3278</v>
+      </c>
+      <c r="C223" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="4" t="s">
+        <v>3279</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>3280</v>
+      </c>
+      <c r="C224" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C225" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="4" t="s">
+        <v>3283</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>3284</v>
+      </c>
+      <c r="C226" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="4" t="s">
+        <v>3285</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>3286</v>
+      </c>
+      <c r="C227" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="4" t="s">
+        <v>3287</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>3288</v>
+      </c>
+      <c r="C228" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="4" t="s">
+        <v>3289</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>3290</v>
+      </c>
+      <c r="C229" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="4" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>3292</v>
+      </c>
+      <c r="C230" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" s="4" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>3294</v>
+      </c>
+      <c r="C231" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="4" t="s">
+        <v>3295</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>3296</v>
+      </c>
+      <c r="C232" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="4" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B233" s="5"/>
+      <c r="C233" s="5"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="4" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>3299</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="4" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="4" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="4" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>3305</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="4" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="4" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>3309</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="4" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B240" s="5"/>
+      <c r="C240" s="5"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="4" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B241" s="5"/>
+      <c r="C241" s="5"/>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="4" t="s">
+        <v>3312</v>
+      </c>
+      <c r="B242" s="5"/>
+      <c r="C242" s="5"/>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="4" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B243" s="5"/>
+      <c r="C243" s="5"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="4" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B244" s="5"/>
+      <c r="C244" s="5"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="4" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B245" s="5"/>
+      <c r="C245" s="5"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="4" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>3317</v>
+      </c>
+      <c r="C246" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" s="4" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B247" s="5"/>
+      <c r="C247" s="5"/>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" s="4" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B248" s="5"/>
+      <c r="C248" s="5"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" s="4" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>3321</v>
+      </c>
+      <c r="C249" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" s="4" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>3323</v>
+      </c>
+      <c r="C250" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" s="4" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>3325</v>
+      </c>
+      <c r="C251" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" s="4" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C252" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" s="4" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>3328</v>
+      </c>
+      <c r="C253" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" s="4" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C254" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="B255" s="5" t="s">
+        <v>3332</v>
+      </c>
+      <c r="C255" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" s="4" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>3334</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" s="4" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B257" s="5" t="s">
+        <v>3336</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" s="4" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>3338</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="4" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>3340</v>
+      </c>
+      <c r="C259" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" s="4" t="s">
+        <v>3341</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>3342</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B261" s="5"/>
+      <c r="C261" s="5"/>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="4" t="s">
+        <v>3343</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>3344</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="4" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C263" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" s="4" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>3348</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="4" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" s="4" t="s">
+        <v>3350</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>3351</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="4" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B267" s="5" t="s">
+        <v>2998</v>
+      </c>
+      <c r="C267" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" s="4" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>3354</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="4" t="s">
+        <v>3355</v>
+      </c>
+      <c r="B269" s="5"/>
+      <c r="C269" s="5"/>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="4" t="s">
+        <v>3356</v>
+      </c>
+      <c r="B270" s="5"/>
+      <c r="C270" s="5"/>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="4" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B271" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="4" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>3008</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" s="4" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>3360</v>
+      </c>
+      <c r="C273" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" s="4" t="s">
+        <v>3361</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>3362</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" s="4" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" s="4" t="s">
+        <v>3364</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>3365</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" s="4" t="s">
+        <v>3366</v>
+      </c>
+      <c r="B277" s="5" t="s">
+        <v>3367</v>
+      </c>
+      <c r="C277" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="4" t="s">
+        <v>3368</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>3369</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" s="4" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B279" s="5" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C279" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" s="4" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C280" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" s="4" t="s">
+        <v>3374</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C281" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" s="4" t="s">
+        <v>3376</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C282" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" s="4" t="s">
+        <v>3378</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C283" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="4" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="4" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>3383</v>
+      </c>
+      <c r="C285" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="4" t="s">
+        <v>3384</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>3385</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="4" t="s">
+        <v>3386</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C287" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="4" t="s">
+        <v>3388</v>
+      </c>
+      <c r="B288" s="5"/>
+      <c r="C288" s="5"/>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="4" t="s">
+        <v>3389</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>3390</v>
+      </c>
+      <c r="C289" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="4" t="s">
+        <v>3391</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>3392</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A290" xr:uid="{F8F58C34-D174-0941-8CA4-E78200493E15}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new maps and phylogeny plots
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08979F97-21EE-E24D-9026-FBEDEC5EC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C754CA-9553-4F43-8C02-0B6A93F903F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="36860" yWindow="-6140" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="3393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="3394">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -10230,6 +10230,9 @@
   </si>
   <si>
     <t>Urosolenia longiseta</t>
+  </si>
+  <si>
+    <t>Eustigmatales</t>
   </si>
 </sst>
 </file>
@@ -23126,8 +23129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D62748D-0C36-F54F-B414-4585403A25D9}">
   <dimension ref="A1:B553"/>
   <sheetViews>
-    <sheetView topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="A256" sqref="A256"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24573,7 +24576,7 @@
         <v>762</v>
       </c>
       <c r="B180" t="s">
-        <v>446</v>
+        <v>316</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -27570,7 +27573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716ADC0-6E42-9D4D-83DC-88C472B153C8}">
   <dimension ref="A1:A78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -27978,8 +27981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}">
   <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29369,7 +29372,7 @@
         <v>446</v>
       </c>
       <c r="B173" t="s">
-        <v>420</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added in fgs for zoo
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C754CA-9553-4F43-8C02-0B6A93F903F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F723D17-5F81-0B4C-BD38-B69EE78F1780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="-6140" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="36860" yWindow="-6140" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="3394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5891" uniqueCount="3395">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -10233,6 +10233,9 @@
   </si>
   <si>
     <t>Eustigmatales</t>
+  </si>
+  <si>
+    <t>Goniochloridales</t>
   </si>
 </sst>
 </file>
@@ -23129,8 +23132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D62748D-0C36-F54F-B414-4585403A25D9}">
   <dimension ref="A1:B553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23896,7 +23899,7 @@
         <v>389</v>
       </c>
       <c r="B95" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -27979,10 +27982,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}">
-  <dimension ref="A1:B189"/>
+  <dimension ref="A1:B190"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29501,6 +29504,14 @@
       </c>
       <c r="B189" t="s">
         <v>2930</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>390</v>
+      </c>
+      <c r="B190" t="s">
+        <v>3394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Need to fix all the outliers, I think somthing weird is going on with kremer
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F723D17-5F81-0B4C-BD38-B69EE78F1780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9825C3F-D73B-544F-9A68-9F742A08288C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="-6140" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" activeTab="6" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5891" uniqueCount="3395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5911" uniqueCount="3401">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -10236,6 +10236,24 @@
   </si>
   <si>
     <t>Goniochloridales</t>
+  </si>
+  <si>
+    <t>Gyromitus (genus in subkingdom SAR)</t>
+  </si>
+  <si>
+    <t>Pyramimonadales</t>
+  </si>
+  <si>
+    <t>Pyramimonadophyceae</t>
+  </si>
+  <si>
+    <t>Sphaerastrum fockii</t>
+  </si>
+  <si>
+    <t>Sorastrum</t>
+  </si>
+  <si>
+    <t>Hydrodictyaceae</t>
   </si>
 </sst>
 </file>
@@ -27984,7 +28002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}">
   <dimension ref="A1:B190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+    <sheetView topLeftCell="A153" workbookViewId="0">
       <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
@@ -29522,10 +29540,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E5C4F8-1C01-BF42-B724-4F4BDD8AA479}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30645,6 +30663,76 @@
         <v>2941</v>
       </c>
       <c r="L30" t="s">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3395</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2731</v>
+      </c>
+      <c r="C31">
+        <v>5653993</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2944</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2731</v>
+      </c>
+      <c r="G31" t="s">
+        <v>616</v>
+      </c>
+      <c r="H31" t="s">
+        <v>3396</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3397</v>
+      </c>
+      <c r="J31" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" t="s">
+        <v>2941</v>
+      </c>
+      <c r="L31" t="s">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>3398</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C32">
+        <v>251731</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2944</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3399</v>
+      </c>
+      <c r="G32" t="s">
+        <v>3400</v>
+      </c>
+      <c r="H32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" t="s">
+        <v>2941</v>
+      </c>
+      <c r="L32" t="s">
         <v>2940</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated all taxonomy and graphs with zooplankton data
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9825C3F-D73B-544F-9A68-9F742A08288C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF90259B-3907-D147-9D8B-1C78F074CDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" activeTab="6" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
   <sheets>
     <sheet name="special_characters" sheetId="33" r:id="rId1"/>
     <sheet name="cleaned" sheetId="47" r:id="rId2"/>
     <sheet name="resolve" sheetId="57" r:id="rId3"/>
     <sheet name="family" sheetId="58" r:id="rId4"/>
-    <sheet name="not_genus" sheetId="55" r:id="rId5"/>
-    <sheet name="order" sheetId="59" r:id="rId6"/>
-    <sheet name="multi_updates" sheetId="60" r:id="rId7"/>
-    <sheet name="cleaned_groups" sheetId="61" r:id="rId8"/>
+    <sheet name="order" sheetId="59" r:id="rId5"/>
+    <sheet name="not_genus" sheetId="55" r:id="rId6"/>
+    <sheet name="non_plankton_multi_check" sheetId="62" r:id="rId7"/>
+    <sheet name="multi_updates" sheetId="60" r:id="rId8"/>
+    <sheet name="cleaned_groups" sheetId="61" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">cleaned_groups!$A$1:$A$290</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">cleaned_groups!$A$1:$A$290</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">family!$B$1:$B$554</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">multi_updates!$K$1:$K$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">order!$B$1:$B$189</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">multi_updates!$K$1:$K$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">order!$B$1:$B$189</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">resolve!$B$1:$B$487</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">special_characters!$B$1:$B$137</definedName>
   </definedNames>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5911" uniqueCount="3401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5959" uniqueCount="3410">
   <si>
     <t>original.taxa.name</t>
   </si>
@@ -10254,6 +10255,33 @@
   </si>
   <si>
     <t>Hydrodictyaceae</t>
+  </si>
+  <si>
+    <t>Pseudophormidium ssp</t>
+  </si>
+  <si>
+    <t>diacyclops bicuspidatus odessanus</t>
+  </si>
+  <si>
+    <t>Diacyclops odessanus</t>
+  </si>
+  <si>
+    <t>Sphaerellopsis</t>
+  </si>
+  <si>
+    <t>Vitreochlamys</t>
+  </si>
+  <si>
+    <t>Brachionus (genus in Opisthokonta)</t>
+  </si>
+  <si>
+    <t>Monogononta</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Gastropidae</t>
   </si>
 </sst>
 </file>
@@ -10663,7 +10691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8595BD-503B-484E-A54B-56E3A4EBC765}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
@@ -11897,10 +11925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286B08F2-9C4E-3A43-A7E5-D98B8AC33438}">
-  <dimension ref="A1:C665"/>
+  <dimension ref="A1:C666"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="A316" sqref="A316"/>
+    <sheetView topLeftCell="A651" workbookViewId="0">
+      <selection activeCell="B672" sqref="B672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19225,6 +19253,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A666" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B666" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C666" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19232,10 +19271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CDAB4C-F5FA-4849-9657-ED9D68F63DEF}">
-  <dimension ref="A1:B487"/>
+  <dimension ref="A1:B488"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A466" workbookViewId="0">
+      <selection activeCell="D478" sqref="D478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23138,6 +23177,14 @@
       </c>
       <c r="B487" t="s">
         <v>1693</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" t="s">
+        <v>3402</v>
+      </c>
+      <c r="B488" t="s">
+        <v>3403</v>
       </c>
     </row>
   </sheetData>
@@ -27591,414 +27638,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716ADC0-6E42-9D4D-83DC-88C472B153C8}">
-  <dimension ref="A1:A78"/>
-  <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2790</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>2752</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>2753</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>2754</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>2759</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>2787</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>2737</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>2738</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>2789</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>2756</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>2836</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>2837</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>2838</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>2839</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>2840</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>2841</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>2842</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>2843</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>2845</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>2846</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>2847</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>2851</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>2852</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7EC72-1B09-7F46-82E1-09C009C1FA6A}">
   <dimension ref="A1:B190"/>
   <sheetViews>
@@ -29538,12 +29177,551 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716ADC0-6E42-9D4D-83DC-88C472B153C8}">
+  <dimension ref="A1:A79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2752</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>2759</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>2738</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>2789</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAECDCE5-0B93-5046-8672-FD134107A566}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2914</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2876</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2878</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2877</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2879</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2881</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3404</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C2">
+        <v>28980</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2944</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3404</v>
+      </c>
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2941</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C3">
+        <v>836111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2944</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2861</v>
+      </c>
+      <c r="G3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2942</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2942</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E5C4F8-1C01-BF42-B724-4F4BDD8AA479}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30736,17 +30914,51 @@
         <v>2940</v>
       </c>
     </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>2758</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3406</v>
+      </c>
+      <c r="C33">
+        <v>471702</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2945</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3406</v>
+      </c>
+      <c r="G33" t="s">
+        <v>221</v>
+      </c>
+      <c r="H33" t="s">
+        <v>220</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3407</v>
+      </c>
+      <c r="J33" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" t="s">
+        <v>3408</v>
+      </c>
+      <c r="L33" t="s">
+        <v>2940</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="K1:K30" xr:uid="{C5E5C4F8-1C01-BF42-B724-4F4BDD8AA479}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F58C34-D174-0941-8CA4-E78200493E15}">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A175" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying to get the log stuff looking better, idk if it has worked
</commit_message>
<xml_diff>
--- a/Raw_data/manual_taxonomy.xlsx
+++ b/Raw_data/manual_taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF90259B-3907-D147-9D8B-1C78F074CDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10DAD1D-CE8E-564D-AD86-A7E23D40FCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{871A196B-DDDF-3A4F-9D63-58F84D4139DF}"/>
   </bookViews>
@@ -29182,7 +29182,7 @@
   <dimension ref="A1:A79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>